<commit_message>
Added delete function for xlsx functions
</commit_message>
<xml_diff>
--- a/server/xlsx/data.xlsx
+++ b/server/xlsx/data.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -410,65 +410,13 @@
       <c r="D2" t="str">
         <v>jim company</v>
       </c>
-      <c r="E2">
-        <v>1628548313164</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Apple</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Its not real</v>
-      </c>
-      <c r="D3" t="str">
-        <v>jim company</v>
-      </c>
-      <c r="E3">
-        <v>1628548447127</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Apple</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Its not real</v>
-      </c>
-      <c r="D4" t="str">
-        <v>jim company</v>
-      </c>
-      <c r="E4" t="str">
-        <v>Mon Aug 09 2021</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Apple</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Its not real</v>
-      </c>
-      <c r="D5" t="str">
-        <v>jim company</v>
-      </c>
-      <c r="E5" t="str">
-        <v>2021-08-09T22:35:52.023Z</v>
+      <c r="E2" t="str">
+        <v>2021-08-12T00:01:21.334Z</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added patch functionality for xlsx functions
</commit_message>
<xml_diff>
--- a/server/xlsx/data.xlsx
+++ b/server/xlsx/data.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -402,21 +402,38 @@
         <v>0</v>
       </c>
       <c r="B2" t="str">
-        <v>Apple</v>
+        <v>Aple</v>
       </c>
       <c r="C2" t="str">
-        <v>Its not real</v>
+        <v>Real</v>
       </c>
       <c r="D2" t="str">
-        <v>jim company</v>
+        <v>COButts</v>
       </c>
       <c r="E2" t="str">
         <v>2021-08-12T00:01:21.334Z</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Mommy</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Fake</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Butts</v>
+      </c>
+      <c r="E3" t="str">
+        <v>2021-08-12T16:04:45.663Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added status and country and city to server model
</commit_message>
<xml_diff>
--- a/server/xlsx/data.xlsx
+++ b/server/xlsx/data.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -396,6 +396,18 @@
       <c r="E1" t="str">
         <v>applyDate</v>
       </c>
+      <c r="F1" t="str">
+        <v>status</v>
+      </c>
+      <c r="G1" t="str">
+        <v>statusId</v>
+      </c>
+      <c r="H1" t="str">
+        <v>country</v>
+      </c>
+      <c r="I1" t="str">
+        <v>city</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
@@ -431,9 +443,84 @@
         <v>2021-08-12T16:04:45.663Z</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="str">
+        <v>gger</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Realsdasd</v>
+      </c>
+      <c r="D4" t="str">
+        <v>asda</v>
+      </c>
+      <c r="E4" t="str">
+        <v>2021-09-06T21:32:47.954Z</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Sent</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="str">
+        <v>gger</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Realsdasd</v>
+      </c>
+      <c r="D5" t="str">
+        <v>asda</v>
+      </c>
+      <c r="E5" t="str">
+        <v>2021-09-06T21:35:48.008Z</v>
+      </c>
+      <c r="F5" t="str">
+        <v>Sent</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="str">
+        <v>gger</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Realsdasd</v>
+      </c>
+      <c r="D6" t="str">
+        <v>asda</v>
+      </c>
+      <c r="E6" t="str">
+        <v>2021-09-06T21:36:51.238Z</v>
+      </c>
+      <c r="F6" t="str">
+        <v>Sent</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="str">
+        <v>canada</v>
+      </c>
+      <c r="I6" t="str">
+        <v>toronto</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added custom error messages for incomplete but required fields
</commit_message>
<xml_diff>
--- a/server/xlsx/data.xlsx
+++ b/server/xlsx/data.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -518,9 +518,67 @@
         <v>toronto</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="str">
+        <v/>
+      </c>
+      <c r="C7" t="str">
+        <v/>
+      </c>
+      <c r="D7" t="str">
+        <v/>
+      </c>
+      <c r="E7" t="str">
+        <v>2021-09-07T12:22:19.891Z</v>
+      </c>
+      <c r="F7" t="str">
+        <v>Sent</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="str">
+        <v/>
+      </c>
+      <c r="I7" t="str">
+        <v>s</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="str">
+        <v>wer</v>
+      </c>
+      <c r="C8" t="str">
+        <v>sd</v>
+      </c>
+      <c r="D8" t="str">
+        <v/>
+      </c>
+      <c r="E8" t="str">
+        <v>2021-09-07T12:31:45.226Z</v>
+      </c>
+      <c r="F8" t="str">
+        <v>Sent</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" t="str">
+        <v/>
+      </c>
+      <c r="I8" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Separating application table and form
</commit_message>
<xml_diff>
--- a/server/xlsx/data.xlsx
+++ b/server/xlsx/data.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -576,9 +576,96 @@
         <v/>
       </c>
     </row>
+    <row r="9">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Big boy</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Biggest boy arouund</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Canada</v>
+      </c>
+      <c r="E9" t="str">
+        <v>2021-10-11T13:31:41.740Z</v>
+      </c>
+      <c r="F9" t="str">
+        <v>Sent</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="str">
+        <v>AD</v>
+      </c>
+      <c r="I9" t="str">
+        <v>los santos</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="str">
+        <v>My lovely Job</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Tiny miney einie weenie time town</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Google</v>
+      </c>
+      <c r="E10" t="str">
+        <v>2021-10-11T13:40:00.771Z</v>
+      </c>
+      <c r="F10" t="str">
+        <v>Sent</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" t="str">
+        <v>AI</v>
+      </c>
+      <c r="I10" t="str">
+        <v>asdas</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="str">
+        <v>s</v>
+      </c>
+      <c r="C11" t="str">
+        <v>d  dasdasd</v>
+      </c>
+      <c r="D11" t="str">
+        <v>asdad</v>
+      </c>
+      <c r="E11" t="str">
+        <v>2021-10-11T13:44:03.679Z</v>
+      </c>
+      <c r="F11" t="str">
+        <v>Sent</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" t="str">
+        <v>Angola</v>
+      </c>
+      <c r="I11" t="str">
+        <v>ASD</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added sort and put app form in table row
</commit_message>
<xml_diff>
--- a/server/xlsx/data.xlsx
+++ b/server/xlsx/data.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -428,24 +428,30 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="str">
-        <v>Mommy</v>
+        <v>gger</v>
       </c>
       <c r="C3" t="str">
-        <v>Fake</v>
+        <v>Realsdasd</v>
       </c>
       <c r="D3" t="str">
-        <v>Butts</v>
+        <v>asda</v>
       </c>
       <c r="E3" t="str">
-        <v>2021-08-12T16:04:45.663Z</v>
+        <v>2021-09-06T21:32:47.954Z</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Sent</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" t="str">
         <v>gger</v>
@@ -457,7 +463,7 @@
         <v>asda</v>
       </c>
       <c r="E4" t="str">
-        <v>2021-09-06T21:32:47.954Z</v>
+        <v>2021-09-06T21:35:48.008Z</v>
       </c>
       <c r="F4" t="str">
         <v>Sent</v>
@@ -468,7 +474,7 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="str">
         <v>gger</v>
@@ -480,7 +486,7 @@
         <v>asda</v>
       </c>
       <c r="E5" t="str">
-        <v>2021-09-06T21:35:48.008Z</v>
+        <v>2021-09-06T21:36:51.238Z</v>
       </c>
       <c r="F5" t="str">
         <v>Sent</v>
@@ -488,184 +494,16 @@
       <c r="G5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="str">
-        <v>gger</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Realsdasd</v>
-      </c>
-      <c r="D6" t="str">
-        <v>asda</v>
-      </c>
-      <c r="E6" t="str">
-        <v>2021-09-06T21:36:51.238Z</v>
-      </c>
-      <c r="F6" t="str">
-        <v>Sent</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6" t="str">
+      <c r="H5" t="str">
         <v>canada</v>
       </c>
-      <c r="I6" t="str">
+      <c r="I5" t="str">
         <v>toronto</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="str">
-        <v/>
-      </c>
-      <c r="C7" t="str">
-        <v/>
-      </c>
-      <c r="D7" t="str">
-        <v/>
-      </c>
-      <c r="E7" t="str">
-        <v>2021-09-07T12:22:19.891Z</v>
-      </c>
-      <c r="F7" t="str">
-        <v>Sent</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7" t="str">
-        <v/>
-      </c>
-      <c r="I7" t="str">
-        <v>s</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="str">
-        <v>wer</v>
-      </c>
-      <c r="C8" t="str">
-        <v>sd</v>
-      </c>
-      <c r="D8" t="str">
-        <v/>
-      </c>
-      <c r="E8" t="str">
-        <v>2021-09-07T12:31:45.226Z</v>
-      </c>
-      <c r="F8" t="str">
-        <v>Sent</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8" t="str">
-        <v/>
-      </c>
-      <c r="I8" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Big boy</v>
-      </c>
-      <c r="C9" t="str">
-        <v>Biggest boy arouund</v>
-      </c>
-      <c r="D9" t="str">
-        <v>Canada</v>
-      </c>
-      <c r="E9" t="str">
-        <v>2021-10-11T13:31:41.740Z</v>
-      </c>
-      <c r="F9" t="str">
-        <v>Sent</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9" t="str">
-        <v>AD</v>
-      </c>
-      <c r="I9" t="str">
-        <v>los santos</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="str">
-        <v>My lovely Job</v>
-      </c>
-      <c r="C10" t="str">
-        <v>Tiny miney einie weenie time town</v>
-      </c>
-      <c r="D10" t="str">
-        <v>Google</v>
-      </c>
-      <c r="E10" t="str">
-        <v>2021-10-11T13:40:00.771Z</v>
-      </c>
-      <c r="F10" t="str">
-        <v>Sent</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10" t="str">
-        <v>AI</v>
-      </c>
-      <c r="I10" t="str">
-        <v>asdas</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="str">
-        <v>s</v>
-      </c>
-      <c r="C11" t="str">
-        <v>d  dasdasd</v>
-      </c>
-      <c r="D11" t="str">
-        <v>asdad</v>
-      </c>
-      <c r="E11" t="str">
-        <v>2021-10-11T13:44:03.679Z</v>
-      </c>
-      <c r="F11" t="str">
-        <v>Sent</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11" t="str">
-        <v>Angola</v>
-      </c>
-      <c r="I11" t="str">
-        <v>ASD</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Played around with form
</commit_message>
<xml_diff>
--- a/server/xlsx/data.xlsx
+++ b/server/xlsx/data.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -396,18 +396,6 @@
       <c r="E1" t="str">
         <v>applyDate</v>
       </c>
-      <c r="F1" t="str">
-        <v>status</v>
-      </c>
-      <c r="G1" t="str">
-        <v>statusId</v>
-      </c>
-      <c r="H1" t="str">
-        <v>country</v>
-      </c>
-      <c r="I1" t="str">
-        <v>city</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2">
@@ -426,84 +414,9 @@
         <v>2021-08-12T00:01:21.334Z</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="str">
-        <v>gger</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Realsdasd</v>
-      </c>
-      <c r="D3" t="str">
-        <v>asda</v>
-      </c>
-      <c r="E3" t="str">
-        <v>2021-09-06T21:32:47.954Z</v>
-      </c>
-      <c r="F3" t="str">
-        <v>Sent</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="str">
-        <v>gger</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Realsdasd</v>
-      </c>
-      <c r="D4" t="str">
-        <v>asda</v>
-      </c>
-      <c r="E4" t="str">
-        <v>2021-09-06T21:35:48.008Z</v>
-      </c>
-      <c r="F4" t="str">
-        <v>Sent</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="str">
-        <v>gger</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Realsdasd</v>
-      </c>
-      <c r="D5" t="str">
-        <v>asda</v>
-      </c>
-      <c r="E5" t="str">
-        <v>2021-09-06T21:36:51.238Z</v>
-      </c>
-      <c r="F5" t="str">
-        <v>Sent</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5" t="str">
-        <v>canada</v>
-      </c>
-      <c r="I5" t="str">
-        <v>toronto</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Small table and form changes
</commit_message>
<xml_diff>
--- a/server/xlsx/data.xlsx
+++ b/server/xlsx/data.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -396,27 +396,80 @@
       <c r="E1" t="str">
         <v>applyDate</v>
       </c>
+      <c r="F1" t="str">
+        <v>status</v>
+      </c>
+      <c r="G1" t="str">
+        <v>statusId</v>
+      </c>
+      <c r="H1" t="str">
+        <v>country</v>
+      </c>
+      <c r="I1" t="str">
+        <v>city</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="str">
-        <v>Aple</v>
+        <v>Fake Job</v>
       </c>
       <c r="C2" t="str">
-        <v>Real</v>
+        <v>It isnt real, you are paid $150,000 CAD to do nothing.</v>
       </c>
       <c r="D2" t="str">
-        <v>COButts</v>
+        <v>Impossible Inc</v>
       </c>
       <c r="E2" t="str">
-        <v>2021-08-12T00:01:21.334Z</v>
+        <v>2021-10-18T02:55:38.252Z</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Sent</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="str">
+        <v>Canada</v>
+      </c>
+      <c r="I2" t="str">
+        <v>Niagara on the Lake</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Also fake</v>
+      </c>
+      <c r="C3" t="str">
+        <v xml:space="preserve">This is is also not real but it pays nothing </v>
+      </c>
+      <c r="D3" t="str">
+        <v>Moo Moo Enterprises</v>
+      </c>
+      <c r="E3" t="str">
+        <v>2021-10-18T02:57:10.079Z</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Sent</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="str">
+        <v>Antarctica</v>
+      </c>
+      <c r="I3" t="str">
+        <v>Godrich</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>